<commit_message>
Lowered stated sugar content.
</commit_message>
<xml_diff>
--- a/SimpleManuals/Nutrition/cookies.xlsx
+++ b/SimpleManuals/Nutrition/cookies.xlsx
@@ -1,25 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Documents\social\nutrition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\18-09-19 Document structure\personal\Programming\git\PublicCodeLibrary\SimpleManuals\Nutrition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146B943D-7DCA-4513-A08E-6E2D098046EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC3E3B1-0513-459F-A8BF-CD81FB515CFF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9225" xr2:uid="{1DA990A8-7916-45FE-A773-58C6EE97C744}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{1DA990A8-7916-45FE-A773-58C6EE97C744}"/>
   </bookViews>
   <sheets>
     <sheet name="Meals" sheetId="1" r:id="rId1"/>
     <sheet name="Ingredients" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -558,7 +563,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C1" sqref="B1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,11 +633,11 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <f>E3/G3*(IF(ISBLANK(H3),I3,H3))</f>
-        <v>200</v>
+        <f t="shared" ref="C3:C14" si="0">E3/G3*(IF(ISBLANK(H3),I3,H3))</f>
+        <v>150</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f>(IF(ISBLANK(H3),I$1,H$1))</f>
+        <f t="shared" ref="D3:D14" si="1">(IF(ISBLANK(H3),I$1,H$1))</f>
         <v>gram</v>
       </c>
       <c r="E3">
@@ -645,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -656,11 +661,11 @@
         <v>17</v>
       </c>
       <c r="C4" s="2">
-        <f>E4/G4*(IF(ISBLANK(H4),I4,H4))</f>
+        <f t="shared" si="0"/>
         <v>170.49600000000001</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f>(IF(ISBLANK(H4),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E4">
@@ -687,11 +692,11 @@
         <v>22</v>
       </c>
       <c r="C5" s="2">
-        <f>E5/G5*(IF(ISBLANK(H5),I5,H5))</f>
+        <f t="shared" si="0"/>
         <v>56.5</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>(IF(ISBLANK(H5),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E5">
@@ -718,11 +723,11 @@
         <v>23</v>
       </c>
       <c r="C6" s="2">
-        <f>E6/G6*(IF(ISBLANK(H6),I6,H6))</f>
+        <f t="shared" si="0"/>
         <v>325</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>(IF(ISBLANK(H6),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E6">
@@ -749,11 +754,11 @@
         <v>18</v>
       </c>
       <c r="C7" s="2">
-        <f>E7/G7*(IF(ISBLANK(H7),I7,H7))</f>
+        <f t="shared" si="0"/>
         <v>59.15</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f>(IF(ISBLANK(H7),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E7">
@@ -780,11 +785,11 @@
         <v>19</v>
       </c>
       <c r="C8" s="2">
-        <f>E8/G8*(IF(ISBLANK(H8),I8,H8))</f>
+        <f t="shared" si="0"/>
         <v>2.1</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>(IF(ISBLANK(H8),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E8">
@@ -811,11 +816,11 @@
         <v>20</v>
       </c>
       <c r="C9" s="2">
-        <f>E9/G9*(IF(ISBLANK(H9),I9,H9))</f>
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>(IF(ISBLANK(H9),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E9">
@@ -842,11 +847,11 @@
         <v>24</v>
       </c>
       <c r="C10" s="2">
-        <f>E10/G10*(IF(ISBLANK(H10),I10,H10))</f>
+        <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>(IF(ISBLANK(H10),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E10">
@@ -870,11 +875,11 @@
         <v>25</v>
       </c>
       <c r="C11" s="2">
-        <f>E11/G11*(IF(ISBLANK(H11),I11,H11))</f>
+        <f t="shared" si="0"/>
         <v>2.4</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f>(IF(ISBLANK(H11),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E11">
@@ -901,11 +906,11 @@
         <v>21</v>
       </c>
       <c r="C12" s="2">
-        <f>E12/G12*(IF(ISBLANK(H12),I12,H12))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>(IF(ISBLANK(H12),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>ml</v>
       </c>
       <c r="E12">
@@ -926,11 +931,11 @@
         <v>26</v>
       </c>
       <c r="C13" s="2">
-        <f>E13/G13*(IF(ISBLANK(H13),I13,H13))</f>
+        <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
       <c r="D13" s="2" t="str">
-        <f>(IF(ISBLANK(H13),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E13">
@@ -957,11 +962,11 @@
         <v>27</v>
       </c>
       <c r="C14" s="2">
-        <f>E14/G14*(IF(ISBLANK(H14),I14,H14))</f>
+        <f t="shared" si="0"/>
         <v>38.295000000000002</v>
       </c>
       <c r="D14" s="2" t="str">
-        <f>(IF(ISBLANK(H14),I$1,H$1))</f>
+        <f t="shared" si="1"/>
         <v>gram</v>
       </c>
       <c r="E14">

</xml_diff>